<commit_message>
add tag to example
</commit_message>
<xml_diff>
--- a/test/test_data/04_worker_incidents.xlsx
+++ b/test/test_data/04_worker_incidents.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandeep/Github/datamart-api/test/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B8DA10-FA8D-954F-B9D5-0B9468B3D8C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E6B8EF-9A34-5047-BBD5-07730437F67F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="66">
   <si>
     <t>dataset</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>http://blablsjskjs.com</t>
+  </si>
+  <si>
+    <t>tag</t>
   </si>
 </sst>
 </file>
@@ -616,10 +619,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G1002"/>
+  <dimension ref="A1:G1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -727,64 +730,53 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="A7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B9" s="10">
         <v>22</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="10">
-        <v>2</v>
-      </c>
-      <c r="F8" s="11">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="1"/>
-      <c r="B9" s="10">
-        <v>47</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="11">
         <v>0</v>
@@ -796,10 +788,10 @@
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="10">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>27</v>
@@ -808,7 +800,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>28</v>
@@ -817,10 +809,10 @@
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="10">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>27</v>
@@ -829,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>28</v>
@@ -838,10 +830,10 @@
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="10">
-        <v>475</v>
+        <v>103</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>
@@ -850,7 +842,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>28</v>
@@ -859,10 +851,10 @@
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="10">
-        <v>782</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>33</v>
+        <v>475</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>27</v>
@@ -880,16 +872,16 @@
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="10">
-        <v>793</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>34</v>
+        <v>782</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E14" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="11">
         <v>0</v>
@@ -901,10 +893,10 @@
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="10">
-        <v>942</v>
+        <v>793</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>27</v>
@@ -922,10 +914,10 @@
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="10">
-        <v>964</v>
+        <v>942</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>27</v>
@@ -943,16 +935,16 @@
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="10">
-        <v>1069</v>
+        <v>964</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="11">
         <v>0</v>
@@ -964,16 +956,16 @@
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="10">
-        <v>1060</v>
+        <v>1069</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" s="11">
         <v>0</v>
@@ -985,16 +977,16 @@
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="10">
-        <v>1102</v>
+        <v>1060</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E19" s="10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F19" s="11">
         <v>0</v>
@@ -1006,16 +998,16 @@
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="10">
-        <v>1281</v>
+        <v>1102</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E20" s="10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F20" s="11">
         <v>0</v>
@@ -1027,19 +1019,19 @@
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="10">
-        <v>1479</v>
+        <v>1281</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="10">
+        <v>1</v>
+      </c>
+      <c r="F21" s="11">
         <v>0</v>
-      </c>
-      <c r="F21" s="11">
-        <v>1</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>28</v>
@@ -1048,19 +1040,19 @@
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="10">
-        <v>1713</v>
+        <v>1479</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E22" s="10">
+        <v>0</v>
+      </c>
+      <c r="F22" s="11">
         <v>1</v>
-      </c>
-      <c r="F22" s="11">
-        <v>0</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>28</v>
@@ -1069,19 +1061,19 @@
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="10">
-        <v>1689</v>
+        <v>1713</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E23" s="10">
+        <v>1</v>
+      </c>
+      <c r="F23" s="11">
         <v>0</v>
-      </c>
-      <c r="F23" s="11">
-        <v>1</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>28</v>
@@ -1090,10 +1082,10 @@
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="10">
-        <v>1931</v>
+        <v>1689</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>27</v>
@@ -1111,10 +1103,10 @@
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
       <c r="B25" s="10">
-        <v>1924</v>
+        <v>1931</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>27</v>
@@ -1132,10 +1124,10 @@
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="B26" s="10">
-        <v>1923</v>
+        <v>1924</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>27</v>
@@ -1153,10 +1145,10 @@
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
       <c r="B27" s="10">
-        <v>1934</v>
+        <v>1923</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>27</v>
@@ -1174,10 +1166,10 @@
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
       <c r="B28" s="10">
-        <v>2143</v>
+        <v>1934</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>27</v>
@@ -1195,10 +1187,10 @@
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
       <c r="B29" s="10">
-        <v>2135</v>
+        <v>2143</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>27</v>
@@ -1216,19 +1208,19 @@
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
       <c r="B30" s="10">
-        <v>2692</v>
+        <v>2135</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E30" s="10">
+        <v>0</v>
+      </c>
+      <c r="F30" s="11">
         <v>1</v>
-      </c>
-      <c r="F30" s="11">
-        <v>0</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>28</v>
@@ -1237,19 +1229,19 @@
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
       <c r="B31" s="10">
-        <v>2623</v>
+        <v>2692</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E31" s="10">
+        <v>1</v>
+      </c>
+      <c r="F31" s="11">
         <v>0</v>
-      </c>
-      <c r="F31" s="11">
-        <v>1</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>28</v>
@@ -1258,19 +1250,19 @@
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
       <c r="B32" s="10">
-        <v>2641</v>
+        <v>2623</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E32" s="10">
+        <v>0</v>
+      </c>
+      <c r="F32" s="11">
         <v>1</v>
-      </c>
-      <c r="F32" s="11">
-        <v>0</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>28</v>
@@ -1279,19 +1271,19 @@
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1"/>
       <c r="B33" s="10">
-        <v>2952</v>
+        <v>2641</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="10">
+        <v>1</v>
+      </c>
+      <c r="F33" s="11">
         <v>0</v>
-      </c>
-      <c r="F33" s="11">
-        <v>1</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>28</v>
@@ -1300,10 +1292,10 @@
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1"/>
       <c r="B34" s="10">
-        <v>2916</v>
+        <v>2952</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>27</v>
@@ -1321,10 +1313,10 @@
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1"/>
       <c r="B35" s="10">
-        <v>3006</v>
+        <v>2916</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>27</v>
@@ -1342,10 +1334,10 @@
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1"/>
       <c r="B36" s="10">
-        <v>2895</v>
+        <v>3006</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>27</v>
@@ -1363,10 +1355,10 @@
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1"/>
       <c r="B37" s="10">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>27</v>
@@ -1375,7 +1367,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>28</v>
@@ -1384,10 +1376,10 @@
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1"/>
       <c r="B38" s="10">
-        <v>2768</v>
+        <v>2896</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>27</v>
@@ -1405,10 +1397,10 @@
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1"/>
       <c r="B39" s="10">
-        <v>2897</v>
+        <v>2768</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>27</v>
@@ -1426,10 +1418,10 @@
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1"/>
       <c r="B40" s="10">
-        <v>2911</v>
+        <v>2897</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>27</v>
@@ -1447,10 +1439,10 @@
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1"/>
       <c r="B41" s="10">
-        <v>2997</v>
+        <v>2911</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>27</v>
@@ -1459,14 +1451,32 @@
         <v>0</v>
       </c>
       <c r="F41" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F42" s="13"/>
+      <c r="A42" s="1"/>
+      <c r="B42" s="10">
+        <v>2997</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" s="10">
+        <v>0</v>
+      </c>
+      <c r="F42" s="11">
+        <v>1</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F43" s="13"/>
@@ -1507,7 +1517,7 @@
     <row r="55" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F55" s="13"/>
     </row>
-    <row r="56" spans="6:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="56" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F56" s="13"/>
     </row>
     <row r="57" spans="6:6" ht="13" x14ac:dyDescent="0.15">
@@ -4347,6 +4357,9 @@
     </row>
     <row r="1002" spans="6:6" ht="13" x14ac:dyDescent="0.15">
       <c r="F1002" s="13"/>
+    </row>
+    <row r="1003" spans="6:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="F1003" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>